<commit_message>
fix bugs dhs. update xls
</commit_message>
<xml_diff>
--- a/auxiliary_data/dhs_dictionary_setcode.xlsx
+++ b/auxiliary_data/dhs_dictionary_setcode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="654">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -288,7 +288,7 @@
     <t xml:space="preserve">argobe</t>
   </si>
   <si>
-    <t xml:space="preserve">autres pays africains sans spcifier</t>
+    <t xml:space="preserve">autres pays africains sans spécifier</t>
   </si>
   <si>
     <t xml:space="preserve">autres pays africans</t>
@@ -378,7 +378,7 @@
     <t xml:space="preserve">foreign/non-congolese</t>
   </si>
   <si>
-    <t xml:space="preserve">gourmantch</t>
+    <t xml:space="preserve">gourmantch,</t>
   </si>
   <si>
     <t xml:space="preserve">gourmantche</t>
@@ -600,7 +600,7 @@
     <t xml:space="preserve">roma (gypsy)</t>
   </si>
   <si>
-    <t xml:space="preserve">sarakol/sonink/marka</t>
+    <t xml:space="preserve">sarakolé/soninké/marka</t>
   </si>
   <si>
     <t xml:space="preserve">sarakole/soninke/marka</t>
@@ -609,16 +609,10 @@
     <t xml:space="preserve">sarkole/soninke/marka</t>
   </si>
   <si>
-    <t xml:space="preserve">snoufo</t>
+    <t xml:space="preserve">s,noufo</t>
   </si>
   <si>
     <t xml:space="preserve">senoufo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snoufo/minianka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">senoufo/minianka</t>
   </si>
   <si>
     <t xml:space="preserve">somalie</t>
@@ -2105,7 +2099,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.24609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2425,7 +2419,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -2434,7 +2428,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,10 +2471,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="5" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -2495,7 +2489,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2582,7 +2576,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="5" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -2594,7 +2588,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>63</v>
@@ -2602,7 +2596,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>45</v>
@@ -2614,7 +2608,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -2626,7 +2620,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -2638,7 +2632,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -2650,7 +2644,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -2659,12 +2653,12 @@
         <v>2001</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>2</v>
@@ -2673,7 +2667,7 @@
         <v>2002</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -2702,7 +2696,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -2778,7 +2772,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="9" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="9" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -2830,10 +2824,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -3526,7 +3520,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="59.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="7" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="7" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -3650,14 +3644,14 @@
   </sheetPr>
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="35.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="35.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -4274,12 +4268,12 @@
         <v>200</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>201</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>76</v>
@@ -4287,10 +4281,10 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,15 +4300,15 @@
         <v>206</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,15 +4316,15 @@
         <v>209</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4359,10 +4353,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,11 +4368,8 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>222</v>
+      <c r="A90" s="1" t="n">
+        <v>999</v>
       </c>
     </row>
   </sheetData>
@@ -4399,7 +4390,7 @@
   </sheetPr>
   <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A130" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4408,1679 +4399,1679 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="C110" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0"/>
       <c r="B130" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0"/>
       <c r="B131" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0"/>
       <c r="B132" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0"/>
       <c r="B133" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0"/>
       <c r="B134" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0"/>
       <c r="B135" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0"/>
       <c r="B136" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0"/>
       <c r="B137" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0"/>
       <c r="B138" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0"/>
       <c r="B139" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0"/>
       <c r="B140" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0"/>
       <c r="B141" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0"/>
       <c r="B142" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0"/>
       <c r="B143" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0"/>
       <c r="B144" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0"/>
       <c r="B145" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0"/>
       <c r="B146" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0"/>
       <c r="B147" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0"/>
       <c r="B148" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0"/>
       <c r="B149" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0"/>
       <c r="B150" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0"/>
       <c r="B151" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0"/>
       <c r="B152" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0"/>
       <c r="B153" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0"/>
       <c r="B154" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0"/>
       <c r="B155" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0"/>
       <c r="B156" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0"/>
       <c r="B157" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -6099,18 +6090,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M71" activeCellId="0" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -6119,313 +6110,313 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
       <c r="B18" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
       <c r="B20" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>145</v>
@@ -6434,7 +6425,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>145</v>
@@ -6443,7 +6434,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>145</v>
@@ -6452,7 +6443,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
       <c r="B38" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>145</v>
@@ -6461,7 +6452,7 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
       <c r="B39" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>145</v>
@@ -6470,7 +6461,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
       <c r="B40" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>145</v>
@@ -6479,7 +6470,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>145</v>
@@ -6488,7 +6479,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>145</v>
@@ -6497,7 +6488,7 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>145</v>
@@ -6506,7 +6497,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>145</v>
@@ -6515,7 +6506,7 @@
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>145</v>
@@ -6524,7 +6515,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>145</v>
@@ -6533,7 +6524,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>145</v>
@@ -6542,64 +6533,64 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6641,79 +6632,79 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
       <c r="B61" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
       <c r="B66" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
       <c r="B67" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>175</v>
@@ -6722,7 +6713,7 @@
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
       <c r="B68" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>175</v>
@@ -6740,7 +6731,7 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
       <c r="B70" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>175</v>
@@ -6749,7 +6740,7 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
       <c r="B71" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>175</v>
@@ -6758,42 +6749,42 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
       <c r="B73" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
       <c r="B74" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
       <c r="B75" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B76" s="1" t="n">
         <v>1</v>
@@ -6804,40 +6795,40 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B77" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B78" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B79" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B80" s="1" t="n">
         <v>6</v>
@@ -6848,13 +6839,18 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B81" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="1" t="n">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -6883,7 +6879,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="10.53"/>
   </cols>
   <sheetData>
@@ -6892,7 +6888,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
change output path, fix nf=nf+1, fix widetable bug
</commit_message>
<xml_diff>
--- a/auxiliary_data/dhs_dictionary_setcode.xlsx
+++ b/auxiliary_data/dhs_dictionary_setcode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="654">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -2095,11 +2095,11 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3644,7 +3644,7 @@
   </sheetPr>
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A57" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B78" activeCellId="0" sqref="B78"/>
     </sheetView>
   </sheetViews>
@@ -6092,8 +6092,8 @@
   </sheetPr>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C82" activeCellId="0" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6843,9 +6843,6 @@
       </c>
       <c r="B81" s="1" t="n">
         <v>9</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update widetable4. add translate
</commit_message>
<xml_diff>
--- a/auxiliary_data/dhs_dictionary_setcode.xlsx
+++ b/auxiliary_data/dhs_dictionary_setcode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="662">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -867,16 +867,16 @@
     <t xml:space="preserve">DominicanRepublic</t>
   </si>
   <si>
-    <t xml:space="preserve">region 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">i  </t>
+    <t xml:space="preserve">region 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
   </si>
   <si>
     <t xml:space="preserve">region i</t>
   </si>
   <si>
-    <t xml:space="preserve">ii </t>
+    <t xml:space="preserve">ii</t>
   </si>
   <si>
     <t xml:space="preserve">region ii</t>
@@ -900,19 +900,19 @@
     <t xml:space="preserve">samana</t>
   </si>
   <si>
-    <t xml:space="preserve">v    </t>
+    <t xml:space="preserve">v</t>
   </si>
   <si>
     <t xml:space="preserve">region v</t>
   </si>
   <si>
-    <t xml:space="preserve">vi  </t>
+    <t xml:space="preserve">vi</t>
   </si>
   <si>
     <t xml:space="preserve">region vi</t>
   </si>
   <si>
-    <t xml:space="preserve">vii </t>
+    <t xml:space="preserve">vii</t>
   </si>
   <si>
     <t xml:space="preserve">region vii</t>
@@ -1681,12 +1681,6 @@
   </si>
   <si>
     <t xml:space="preserve">matabeleland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atl ntico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atlantico</t>
   </si>
   <si>
     <t xml:space="preserve">nord quest</t>
@@ -2133,7 +2127,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2462,7 +2456,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,7 +2517,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2622,7 +2616,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>65</v>
@@ -2630,7 +2624,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>45</v>
@@ -2642,7 +2636,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -2654,7 +2648,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -2666,7 +2660,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -2678,7 +2672,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -2687,12 +2681,12 @@
         <v>2001</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>2</v>
@@ -2701,7 +2695,7 @@
         <v>2002</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -3543,7 +3537,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -4471,10 +4465,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C158"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A158"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6181,7 +6175,9 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0"/>
+      <c r="A155" s="0" t="s">
+        <v>274</v>
+      </c>
       <c r="B155" s="1" t="s">
         <v>550</v>
       </c>
@@ -6190,7 +6186,9 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0"/>
+      <c r="A156" s="0" t="s">
+        <v>357</v>
+      </c>
       <c r="B156" s="1" t="s">
         <v>552</v>
       </c>
@@ -6199,23 +6197,14 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0"/>
+      <c r="A157" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="B157" s="1" t="s">
         <v>554</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -6254,313 +6243,313 @@
         <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
       <c r="B3" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
       <c r="B18" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0"/>
       <c r="B19" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
       <c r="B20" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
       <c r="B21" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
       <c r="B23" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
       <c r="B25" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
       <c r="B27" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
       <c r="B29" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0"/>
       <c r="B31" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
       <c r="B33" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
       <c r="B35" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>152</v>
@@ -6569,7 +6558,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>152</v>
@@ -6578,7 +6567,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0"/>
       <c r="B37" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>152</v>
@@ -6587,7 +6576,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
       <c r="B38" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>152</v>
@@ -6596,7 +6585,7 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
       <c r="B39" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>152</v>
@@ -6605,7 +6594,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
       <c r="B40" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>152</v>
@@ -6614,7 +6603,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>152</v>
@@ -6623,7 +6612,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>152</v>
@@ -6632,7 +6621,7 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
       <c r="B43" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>152</v>
@@ -6641,7 +6630,7 @@
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>152</v>
@@ -6650,7 +6639,7 @@
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0"/>
       <c r="B45" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>152</v>
@@ -6659,7 +6648,7 @@
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>152</v>
@@ -6668,7 +6657,7 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0"/>
       <c r="B47" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>152</v>
@@ -6677,64 +6666,64 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
       <c r="B49" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0"/>
       <c r="B51" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="1" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6776,79 +6765,79 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
       <c r="B61" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0"/>
       <c r="B64" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0"/>
       <c r="B65" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0"/>
       <c r="B66" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0"/>
       <c r="B67" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>182</v>
@@ -6857,7 +6846,7 @@
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0"/>
       <c r="B68" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>182</v>
@@ -6875,7 +6864,7 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
       <c r="B70" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>182</v>
@@ -6884,7 +6873,7 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>
       <c r="B71" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>182</v>
@@ -6893,37 +6882,37 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
       <c r="B72" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0"/>
       <c r="B73" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
       <c r="B74" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0"/>
       <c r="B75" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6945,7 +6934,7 @@
         <v>2</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6956,7 +6945,7 @@
         <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6967,7 +6956,7 @@
         <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7029,7 +7018,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>